<commit_message>
Lots of refactoring, removed JSON support.
</commit_message>
<xml_diff>
--- a/CG_FinalAssignment_EvaluationForm_s1129160_LucasOuwens.xlsx
+++ b/CG_FinalAssignment_EvaluationForm_s1129160_LucasOuwens.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\School\CG_2021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2564B3B-8F23-4614-9F7F-2AE93275F144}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B454E31E-841E-4B93-BA75-1AF124575E99}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27260" yWindow="-970" windowWidth="27370" windowHeight="14890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Evaluation form" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="107">
   <si>
     <t>Knock-out criteria</t>
   </si>
@@ -332,10 +332,28 @@
     <t>Implemented drone mode, switching can be done by using 'v'. You will be transported upon applying it.</t>
   </si>
   <si>
-    <t>Implemented walking mode, uses mouse movement for the camera (so no I/J/K/L) fallthrough is impossible, due to a hard limit.</t>
-  </si>
-  <si>
     <t>Application of strategy pattern for movement controllers, code is documented.</t>
+  </si>
+  <si>
+    <t>three types of shaders (includes the fragment shading aspect): Basic, Lambert and Phong.</t>
+  </si>
+  <si>
+    <t>Skybox, floor</t>
+  </si>
+  <si>
+    <t>Skybox texture, floor grass texture, floor dirt texture</t>
+  </si>
+  <si>
+    <t>s1129160</t>
+  </si>
+  <si>
+    <t>Lucas Ouwens</t>
+  </si>
+  <si>
+    <t>Implemented walking mode, uses mouse movement for the camera (so no I/J/K/L) fallthrough is impossible.</t>
+  </si>
+  <si>
+    <t>tile mesh / floor model, skybox consists of multiple primitive meshes (6 of them)</t>
   </si>
 </sst>
 </file>
@@ -1321,8 +1339,8 @@
   </sheetPr>
   <dimension ref="B2:M36"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A17" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M30" sqref="M30"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1356,14 +1374,18 @@
       <c r="C4" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="E4" s="45"/>
+      <c r="E4" s="45" t="s">
+        <v>103</v>
+      </c>
       <c r="F4" s="46"/>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C5" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="E5" s="40"/>
+      <c r="E5" s="40" t="s">
+        <v>104</v>
+      </c>
       <c r="F5" s="41"/>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.25">
@@ -1497,9 +1519,11 @@
       <c r="K19" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="M19" s="31"/>
-    </row>
-    <row r="20" spans="2:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="M19" s="31" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="20" spans="2:13" ht="45" x14ac:dyDescent="0.25">
       <c r="C20" s="4" t="s">
         <v>85</v>
       </c>
@@ -1517,7 +1541,9 @@
       <c r="K20" s="35" t="s">
         <v>87</v>
       </c>
-      <c r="M20" s="32"/>
+      <c r="M20" s="32" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="21" spans="2:13" ht="30" x14ac:dyDescent="0.25">
       <c r="C21" s="4" t="s">
@@ -1557,7 +1583,9 @@
       <c r="K22" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="M22" s="32"/>
+      <c r="M22" s="32" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="23" spans="2:13" ht="75" x14ac:dyDescent="0.25">
       <c r="C23" s="4" t="s">
@@ -1597,7 +1625,9 @@
       <c r="K24" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="M24" s="32"/>
+      <c r="M24" s="32" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="25" spans="2:13" ht="60" x14ac:dyDescent="0.25">
       <c r="C25" s="4" t="s">
@@ -1618,7 +1648,7 @@
         <v>95</v>
       </c>
       <c r="M25" s="32" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
     </row>
     <row r="26" spans="2:13" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1687,7 +1717,7 @@
         <v>45</v>
       </c>
       <c r="M29" s="28" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="30" spans="2:13" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Progress on CG assignment 3
</commit_message>
<xml_diff>
--- a/CG_FinalAssignment_EvaluationForm_s1129160_LucasOuwens.xlsx
+++ b/CG_FinalAssignment_EvaluationForm_s1129160_LucasOuwens.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\School\CG_2021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B454E31E-841E-4B93-BA75-1AF124575E99}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{855B199E-6AA4-4681-83D9-E6F42E238C98}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-27260" yWindow="-970" windowWidth="27370" windowHeight="14890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Evaluation form" sheetId="1" r:id="rId1"/>
@@ -335,15 +335,9 @@
     <t>Application of strategy pattern for movement controllers, code is documented.</t>
   </si>
   <si>
-    <t>three types of shaders (includes the fragment shading aspect): Basic, Lambert and Phong.</t>
-  </si>
-  <si>
     <t>Skybox, floor</t>
   </si>
   <si>
-    <t>Skybox texture, floor grass texture, floor dirt texture</t>
-  </si>
-  <si>
     <t>s1129160</t>
   </si>
   <si>
@@ -354,6 +348,12 @@
   </si>
   <si>
     <t>tile mesh / floor model, skybox consists of multiple primitive meshes (6 of them)</t>
+  </si>
+  <si>
+    <t>three types of shaders (includes the fragment shading aspect): Basic, Lambert and Phong. The floor uses the phong shader, and the further the tile is from the center, the less shiny it is. The skybox uses the basic shading and the other elements all use lambert shading.</t>
+  </si>
+  <si>
+    <t>floor grass texture, floor dirt texture, the skybox uses  6 unique textures as well. It is very simple to add geometries which can have a texture.</t>
   </si>
 </sst>
 </file>
@@ -1339,8 +1339,8 @@
   </sheetPr>
   <dimension ref="B2:M36"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K30" sqref="K30"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1375,7 +1375,7 @@
         <v>96</v>
       </c>
       <c r="E4" s="45" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F4" s="46"/>
     </row>
@@ -1384,7 +1384,7 @@
         <v>97</v>
       </c>
       <c r="E5" s="40" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F5" s="41"/>
     </row>
@@ -1520,7 +1520,7 @@
         <v>64</v>
       </c>
       <c r="M19" s="31" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="20" spans="2:13" ht="45" x14ac:dyDescent="0.25">
@@ -1542,7 +1542,7 @@
         <v>87</v>
       </c>
       <c r="M20" s="32" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="21" spans="2:13" ht="30" x14ac:dyDescent="0.25">
@@ -1584,7 +1584,7 @@
         <v>57</v>
       </c>
       <c r="M22" s="32" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
     </row>
     <row r="23" spans="2:13" ht="75" x14ac:dyDescent="0.25">
@@ -1607,7 +1607,7 @@
       </c>
       <c r="M23" s="32"/>
     </row>
-    <row r="24" spans="2:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:13" ht="120" x14ac:dyDescent="0.25">
       <c r="C24" s="4" t="s">
         <v>82</v>
       </c>
@@ -1626,7 +1626,7 @@
         <v>81</v>
       </c>
       <c r="M24" s="32" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
     </row>
     <row r="25" spans="2:13" ht="60" x14ac:dyDescent="0.25">
@@ -1648,7 +1648,7 @@
         <v>95</v>
       </c>
       <c r="M25" s="32" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="26" spans="2:13" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1949,32 +1949,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_Flow_SignoffStatus xmlns="e7647ff1-e2f7-42a1-a68c-3c96587cf758" xsi:nil="true"/>
-    <SharedWithUsers xmlns="7178be8b-d0ef-4995-97d9-396f4bad9a56">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010031DCE2413392E94399C66D8B3C6C85EE" ma:contentTypeVersion="15" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="0c2036bf52fce6a572da55f07fac53b0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="e7647ff1-e2f7-42a1-a68c-3c96587cf758" xmlns:ns3="7178be8b-d0ef-4995-97d9-396f4bad9a56" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="46a6dac1cb1c034944cf78d34111dc32" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -2214,33 +2188,33 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{704D0896-41A1-4D8E-B2B4-DAF4537F2CEF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="e7647ff1-e2f7-42a1-a68c-3c96587cf758"/>
-    <ds:schemaRef ds:uri="7178be8b-d0ef-4995-97d9-396f4bad9a56"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{95702B07-5163-4733-93F0-15C1454EB37E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_Flow_SignoffStatus xmlns="e7647ff1-e2f7-42a1-a68c-3c96587cf758" xsi:nil="true"/>
+    <SharedWithUsers xmlns="7178be8b-d0ef-4995-97d9-396f4bad9a56">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{169FD9BA-39C5-40E5-9D02-8D3DF9B0119E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2258,4 +2232,30 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{95702B07-5163-4733-93F0-15C1454EB37E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{704D0896-41A1-4D8E-B2B4-DAF4537F2CEF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="e7647ff1-e2f7-42a1-a68c-3c96587cf758"/>
+    <ds:schemaRef ds:uri="7178be8b-d0ef-4995-97d9-396f4bad9a56"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added a lot of models into the world, will evt. refactor some of them.
</commit_message>
<xml_diff>
--- a/CG_FinalAssignment_EvaluationForm_s1129160_LucasOuwens.xlsx
+++ b/CG_FinalAssignment_EvaluationForm_s1129160_LucasOuwens.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\School\CG_2021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EC13670-18FC-4671-8539-9615CCAACA29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C75379E-E83B-4DF6-A469-56A00489E3EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -335,9 +335,6 @@
     <t>Application of strategy pattern for movement controllers, code is documented.</t>
   </si>
   <si>
-    <t>Skybox, floor</t>
-  </si>
-  <si>
     <t>s1129160</t>
   </si>
   <si>
@@ -347,16 +344,19 @@
     <t>Implemented walking mode, uses mouse movement for the camera (so no I/J/K/L) fallthrough is impossible.</t>
   </si>
   <si>
-    <t>three types of shaders (includes the fragment shading aspect): Basic, Lambert and Phong. The floor uses the phong shader, and the further the tile is from the center, the less shiny it is. The skybox uses the basic shading and the other elements all use lambert shading.</t>
-  </si>
-  <si>
-    <t>floor grass texture, floor dirt texture, skybox texture. It is very simple to add geometries which can have a texture.</t>
-  </si>
-  <si>
-    <t>Skybox, house</t>
-  </si>
-  <si>
     <t>Only have a single mesh (but they fill the entire ground). It is also really easy to extend. (just create a new subclass &amp; add it)</t>
+  </si>
+  <si>
+    <t>basic shading on the house, phong shading on the other objects. The floor's shininess becomes higher the closer to the middle you look at it.</t>
+  </si>
+  <si>
+    <t>Skybox, floor, two different trees, two different bushes, a house, a fence with a fence gate, flowers and a couch. You can easily expand the amount of models by writing some code in the geometrybuilder and environmentbuilder.</t>
+  </si>
+  <si>
+    <t>Skybox, floor, two different trees, two different bushes, a house, a fence with a fence gate, a flower and a couch.</t>
+  </si>
+  <si>
+    <t>floor grass texture, floor dirt texture, skybox texture. Multiple textures are easily added by splitting a big model into smaller ones and applying a texture on them separately. Then we can easily group them together using a MeshGrouping</t>
   </si>
 </sst>
 </file>
@@ -1342,8 +1342,8 @@
   </sheetPr>
   <dimension ref="B2:M36"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K29" sqref="K29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1378,7 +1378,7 @@
         <v>96</v>
       </c>
       <c r="E4" s="45" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F4" s="46"/>
     </row>
@@ -1387,7 +1387,7 @@
         <v>97</v>
       </c>
       <c r="E5" s="40" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F5" s="41"/>
     </row>
@@ -1504,7 +1504,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="2:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:13" ht="105" x14ac:dyDescent="0.25">
       <c r="C19" s="4" t="s">
         <v>84</v>
       </c>
@@ -1523,7 +1523,7 @@
         <v>64</v>
       </c>
       <c r="M19" s="31" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
     </row>
     <row r="20" spans="2:13" ht="60" x14ac:dyDescent="0.25">
@@ -1545,10 +1545,10 @@
         <v>87</v>
       </c>
       <c r="M20" s="32" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="21" spans="2:13" ht="30" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="21" spans="2:13" ht="60" x14ac:dyDescent="0.25">
       <c r="C21" s="4" t="s">
         <v>48</v>
       </c>
@@ -1570,7 +1570,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="22" spans="2:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:13" ht="105" x14ac:dyDescent="0.25">
       <c r="C22" s="4" t="s">
         <v>53</v>
       </c>
@@ -1589,7 +1589,7 @@
         <v>57</v>
       </c>
       <c r="M22" s="32" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="23" spans="2:13" ht="75" x14ac:dyDescent="0.25">
@@ -1612,7 +1612,7 @@
       </c>
       <c r="M23" s="32"/>
     </row>
-    <row r="24" spans="2:13" ht="120" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:13" ht="60" x14ac:dyDescent="0.25">
       <c r="C24" s="4" t="s">
         <v>82</v>
       </c>
@@ -1653,7 +1653,7 @@
         <v>95</v>
       </c>
       <c r="M25" s="32" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="26" spans="2:13" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1960,6 +1960,32 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_Flow_SignoffStatus xmlns="e7647ff1-e2f7-42a1-a68c-3c96587cf758" xsi:nil="true"/>
+    <SharedWithUsers xmlns="7178be8b-d0ef-4995-97d9-396f4bad9a56">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010031DCE2413392E94399C66D8B3C6C85EE" ma:contentTypeVersion="15" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="0c2036bf52fce6a572da55f07fac53b0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="e7647ff1-e2f7-42a1-a68c-3c96587cf758" xmlns:ns3="7178be8b-d0ef-4995-97d9-396f4bad9a56" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="46a6dac1cb1c034944cf78d34111dc32" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -2199,33 +2225,33 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{704D0896-41A1-4D8E-B2B4-DAF4537F2CEF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="e7647ff1-e2f7-42a1-a68c-3c96587cf758"/>
+    <ds:schemaRef ds:uri="7178be8b-d0ef-4995-97d9-396f4bad9a56"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_Flow_SignoffStatus xmlns="e7647ff1-e2f7-42a1-a68c-3c96587cf758" xsi:nil="true"/>
-    <SharedWithUsers xmlns="7178be8b-d0ef-4995-97d9-396f4bad9a56">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{95702B07-5163-4733-93F0-15C1454EB37E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{169FD9BA-39C5-40E5-9D02-8D3DF9B0119E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2243,30 +2269,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{95702B07-5163-4733-93F0-15C1454EB37E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{704D0896-41A1-4D8E-B2B4-DAF4537F2CEF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="e7647ff1-e2f7-42a1-a68c-3c96587cf758"/>
-    <ds:schemaRef ds:uri="7178be8b-d0ef-4995-97d9-396f4bad9a56"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Some refinements, proper placing of stuff
</commit_message>
<xml_diff>
--- a/CG_FinalAssignment_EvaluationForm_s1129160_LucasOuwens.xlsx
+++ b/CG_FinalAssignment_EvaluationForm_s1129160_LucasOuwens.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\School\CG_2021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01E4248B-ADAA-40BA-A3C8-DF5C4226D971}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAEC6A0C-5E87-4D9A-91D6-0E1534D52E2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -344,12 +344,6 @@
     <t>Only have a single mesh (but they fill the entire ground). It is also really easy to extend. (just create a new subclass &amp; add it)</t>
   </si>
   <si>
-    <t>basic shading on the house, phong shading on the other objects. The floor's shininess becomes higher the closer to the middle you look at it.</t>
-  </si>
-  <si>
-    <t>Skybox, floor, two different trees, two different bushes, a house, a fence with a fence gate, flowers and a couch. You can easily expand the amount of models by writing some code in the geometrybuilder and environmentbuilder.</t>
-  </si>
-  <si>
     <t>I believe I have made good looking objects, they're pretty creatively made as well.</t>
   </si>
   <si>
@@ -362,7 +356,13 @@
     <t>Skybox, floor, two different trees, two different bushes, a house, a fence with a fence gate, a flower and a couch. I made all the models in the world by myself.</t>
   </si>
   <si>
-    <t>Comments have been placed at their relevant locations, method and variable naming is clear. Note that methods are explained in the .cpp file &amp; not the .h file. This has been the most convenient way for me to add useful comments without adding duplicity.</t>
+    <t>Comments have been placed at their relevant locations, method and variable naming is clear. Note that methods are explained in the .h file &amp; not the .cpp file. This has been the most convenient way for me to add useful comments without adding duplicity.</t>
+  </si>
+  <si>
+    <t>Skybox, floor, two different trees, two different bushes, a house, a fence with a fence gate, a flower and a couch. You can easily expand the amount of models by writing some code in the geometrybuilder and environmentbuilder.</t>
+  </si>
+  <si>
+    <t>basic shading on the house, phong shading on the other objects. The further you are from (12, N, 32) the less shiny the floor is.</t>
   </si>
 </sst>
 </file>
@@ -1348,8 +1348,8 @@
   </sheetPr>
   <dimension ref="B2:M36"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A27" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A21" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M24" sqref="M24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1529,7 +1529,7 @@
         <v>64</v>
       </c>
       <c r="M19" s="31" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
     </row>
     <row r="20" spans="2:13" ht="60" x14ac:dyDescent="0.25">
@@ -1573,7 +1573,7 @@
         <v>49</v>
       </c>
       <c r="M21" s="32" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="22" spans="2:13" ht="150" x14ac:dyDescent="0.25">
@@ -1595,7 +1595,7 @@
         <v>57</v>
       </c>
       <c r="M22" s="32" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="23" spans="2:13" ht="75" x14ac:dyDescent="0.25">
@@ -1637,7 +1637,7 @@
         <v>81</v>
       </c>
       <c r="M24" s="32" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
     </row>
     <row r="25" spans="2:13" ht="60" x14ac:dyDescent="0.25">
@@ -1728,7 +1728,7 @@
         <v>45</v>
       </c>
       <c r="M29" s="28" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="30" spans="2:13" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1750,7 +1750,7 @@
         <v>42</v>
       </c>
       <c r="M30" s="29" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="32" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1835,7 +1835,7 @@
         <v>73</v>
       </c>
       <c r="M35" s="29" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="36" spans="3:13" x14ac:dyDescent="0.25">
@@ -1964,6 +1964,32 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_Flow_SignoffStatus xmlns="e7647ff1-e2f7-42a1-a68c-3c96587cf758" xsi:nil="true"/>
+    <SharedWithUsers xmlns="7178be8b-d0ef-4995-97d9-396f4bad9a56">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010031DCE2413392E94399C66D8B3C6C85EE" ma:contentTypeVersion="15" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="0c2036bf52fce6a572da55f07fac53b0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="e7647ff1-e2f7-42a1-a68c-3c96587cf758" xmlns:ns3="7178be8b-d0ef-4995-97d9-396f4bad9a56" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="46a6dac1cb1c034944cf78d34111dc32" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -2203,33 +2229,33 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{704D0896-41A1-4D8E-B2B4-DAF4537F2CEF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="e7647ff1-e2f7-42a1-a68c-3c96587cf758"/>
+    <ds:schemaRef ds:uri="7178be8b-d0ef-4995-97d9-396f4bad9a56"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_Flow_SignoffStatus xmlns="e7647ff1-e2f7-42a1-a68c-3c96587cf758" xsi:nil="true"/>
-    <SharedWithUsers xmlns="7178be8b-d0ef-4995-97d9-396f4bad9a56">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{95702B07-5163-4733-93F0-15C1454EB37E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{169FD9BA-39C5-40E5-9D02-8D3DF9B0119E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2247,30 +2273,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{95702B07-5163-4733-93F0-15C1454EB37E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{704D0896-41A1-4D8E-B2B4-DAF4537F2CEF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="e7647ff1-e2f7-42a1-a68c-3c96587cf758"/>
-    <ds:schemaRef ds:uri="7178be8b-d0ef-4995-97d9-396f4bad9a56"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Some changes to the excel sheet
</commit_message>
<xml_diff>
--- a/CG_FinalAssignment_EvaluationForm_s1129160_LucasOuwens.xlsx
+++ b/CG_FinalAssignment_EvaluationForm_s1129160_LucasOuwens.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\School\CG_2021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAEC6A0C-5E87-4D9A-91D6-0E1534D52E2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6E9FC0C-2963-4BD2-8C96-C4CF870F8316}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="111">
   <si>
     <t>Knock-out criteria</t>
   </si>
@@ -329,9 +329,6 @@
     <t>Student name</t>
   </si>
   <si>
-    <t>Implemented drone mode, switching can be done by using 'v'. You will be transported upon applying it.</t>
-  </si>
-  <si>
     <t>s1129160</t>
   </si>
   <si>
@@ -363,6 +360,12 @@
   </si>
   <si>
     <t>basic shading on the house, phong shading on the other objects. The further you are from (12, N, 32) the less shiny the floor is.</t>
+  </si>
+  <si>
+    <t>Implemented drone mode, switching can be done by using 'v'. You will be transported upon applying it. You will get a nice overview of the scene, you can move around like a drone (camera moves towards where you are facing incl y-axis.) You can also use Q/E to move up and down if you prefer this.</t>
+  </si>
+  <si>
+    <t>My models look pretty decent, I believe.</t>
   </si>
 </sst>
 </file>
@@ -1348,8 +1351,8 @@
   </sheetPr>
   <dimension ref="B2:M36"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A21" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M24" sqref="M24"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M34" sqref="M34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1384,7 +1387,7 @@
         <v>96</v>
       </c>
       <c r="E4" s="45" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F4" s="46"/>
     </row>
@@ -1393,7 +1396,7 @@
         <v>97</v>
       </c>
       <c r="E5" s="40" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F5" s="41"/>
     </row>
@@ -1529,7 +1532,7 @@
         <v>64</v>
       </c>
       <c r="M19" s="31" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="20" spans="2:13" ht="60" x14ac:dyDescent="0.25">
@@ -1551,7 +1554,7 @@
         <v>87</v>
       </c>
       <c r="M20" s="32" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="21" spans="2:13" ht="75" x14ac:dyDescent="0.25">
@@ -1573,7 +1576,7 @@
         <v>49</v>
       </c>
       <c r="M21" s="32" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="22" spans="2:13" ht="150" x14ac:dyDescent="0.25">
@@ -1595,7 +1598,7 @@
         <v>57</v>
       </c>
       <c r="M22" s="32" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="23" spans="2:13" ht="75" x14ac:dyDescent="0.25">
@@ -1637,7 +1640,7 @@
         <v>81</v>
       </c>
       <c r="M24" s="32" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="25" spans="2:13" ht="60" x14ac:dyDescent="0.25">
@@ -1659,10 +1662,10 @@
         <v>95</v>
       </c>
       <c r="M25" s="32" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="26" spans="2:13" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="26" spans="2:13" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C26" s="4" t="s">
         <v>90</v>
       </c>
@@ -1679,7 +1682,7 @@
       </c>
       <c r="K26" s="48"/>
       <c r="M26" s="33" t="s">
-        <v>98</v>
+        <v>109</v>
       </c>
     </row>
     <row r="28" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1728,7 +1731,7 @@
         <v>45</v>
       </c>
       <c r="M29" s="28" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="30" spans="2:13" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1750,7 +1753,7 @@
         <v>42</v>
       </c>
       <c r="M30" s="29" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="32" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1796,7 +1799,9 @@
         <v>75</v>
       </c>
       <c r="K33" s="39"/>
-      <c r="M33" s="28"/>
+      <c r="M33" s="28" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="34" spans="3:13" ht="30" x14ac:dyDescent="0.25">
       <c r="C34" s="4" t="s">
@@ -1835,7 +1840,7 @@
         <v>73</v>
       </c>
       <c r="M35" s="29" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="36" spans="3:13" x14ac:dyDescent="0.25">
@@ -1873,7 +1878,7 @@
   <dimension ref="C2:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B11"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1964,32 +1969,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_Flow_SignoffStatus xmlns="e7647ff1-e2f7-42a1-a68c-3c96587cf758" xsi:nil="true"/>
-    <SharedWithUsers xmlns="7178be8b-d0ef-4995-97d9-396f4bad9a56">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010031DCE2413392E94399C66D8B3C6C85EE" ma:contentTypeVersion="15" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="0c2036bf52fce6a572da55f07fac53b0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="e7647ff1-e2f7-42a1-a68c-3c96587cf758" xmlns:ns3="7178be8b-d0ef-4995-97d9-396f4bad9a56" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="46a6dac1cb1c034944cf78d34111dc32" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -2229,33 +2208,33 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{704D0896-41A1-4D8E-B2B4-DAF4537F2CEF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="e7647ff1-e2f7-42a1-a68c-3c96587cf758"/>
-    <ds:schemaRef ds:uri="7178be8b-d0ef-4995-97d9-396f4bad9a56"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{95702B07-5163-4733-93F0-15C1454EB37E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_Flow_SignoffStatus xmlns="e7647ff1-e2f7-42a1-a68c-3c96587cf758" xsi:nil="true"/>
+    <SharedWithUsers xmlns="7178be8b-d0ef-4995-97d9-396f4bad9a56">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{169FD9BA-39C5-40E5-9D02-8D3DF9B0119E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2273,4 +2252,30 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{95702B07-5163-4733-93F0-15C1454EB37E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{704D0896-41A1-4D8E-B2B4-DAF4537F2CEF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="e7647ff1-e2f7-42a1-a68c-3c96587cf758"/>
+    <ds:schemaRef ds:uri="7178be8b-d0ef-4995-97d9-396f4bad9a56"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Implemented wave animation for couches
</commit_message>
<xml_diff>
--- a/CG_FinalAssignment_EvaluationForm_s1129160_LucasOuwens.xlsx
+++ b/CG_FinalAssignment_EvaluationForm_s1129160_LucasOuwens.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\School\CG_2021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6E9FC0C-2963-4BD2-8C96-C4CF870F8316}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0CBCBAF-858D-411E-92DD-D444AB26BF50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="112">
   <si>
     <t>Knock-out criteria</t>
   </si>
@@ -366,6 +366,9 @@
   </si>
   <si>
     <t>My models look pretty decent, I believe.</t>
+  </si>
+  <si>
+    <t>Easy to use animation system, just create a subclass, implement the execute method. Then, make a new object out of the animation and set the owner of the animation &amp; register it at the animation manager. Skybox rotates, flower moves up and back down whilst rotating on the y and x axis. Couches have wave animations for seats</t>
   </si>
 </sst>
 </file>
@@ -1351,8 +1354,8 @@
   </sheetPr>
   <dimension ref="B2:M36"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M34" sqref="M34"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1601,7 +1604,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="23" spans="2:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:13" ht="150" x14ac:dyDescent="0.25">
       <c r="C23" s="4" t="s">
         <v>32</v>
       </c>
@@ -1619,7 +1622,9 @@
       <c r="K23" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="M23" s="32"/>
+      <c r="M23" s="32" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="24" spans="2:13" ht="60" x14ac:dyDescent="0.25">
       <c r="C24" s="4" t="s">

</xml_diff>

<commit_message>
Implemented gate toggling animation, bird wings.
</commit_message>
<xml_diff>
--- a/CG_FinalAssignment_EvaluationForm_s1129160_LucasOuwens.xlsx
+++ b/CG_FinalAssignment_EvaluationForm_s1129160_LucasOuwens.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\School\CG_2021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0CBCBAF-858D-411E-92DD-D444AB26BF50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6DBD576-66A1-423B-95A7-09C74CDDC35B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -368,7 +368,7 @@
     <t>My models look pretty decent, I believe.</t>
   </si>
   <si>
-    <t>Easy to use animation system, just create a subclass, implement the execute method. Then, make a new object out of the animation and set the owner of the animation &amp; register it at the animation manager. Skybox rotates, flower moves up and back down whilst rotating on the y and x axis. Couches have wave animations for seats</t>
+    <t xml:space="preserve">Easy to use animation system, just create a subclass, implement the execute method. Then, make a new object out of the animation and set the owner of the animation &amp; register it at the animation manager. Skybox rotates, flower moves up and back down whilst rotating on the y and x axis. Couches have wave animations for seats. Press 'g' to open/cose the gate of the fence, you can stop it from opening or closer further by prematurely pressing 'g' again. </t>
   </si>
 </sst>
 </file>
@@ -1354,8 +1354,8 @@
   </sheetPr>
   <dimension ref="B2:M36"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M23" sqref="M23"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1604,7 +1604,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="23" spans="2:13" ht="150" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:13" ht="195" x14ac:dyDescent="0.25">
       <c r="C23" s="4" t="s">
         <v>32</v>
       </c>
@@ -1974,6 +1974,32 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_Flow_SignoffStatus xmlns="e7647ff1-e2f7-42a1-a68c-3c96587cf758" xsi:nil="true"/>
+    <SharedWithUsers xmlns="7178be8b-d0ef-4995-97d9-396f4bad9a56">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010031DCE2413392E94399C66D8B3C6C85EE" ma:contentTypeVersion="15" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="0c2036bf52fce6a572da55f07fac53b0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="e7647ff1-e2f7-42a1-a68c-3c96587cf758" xmlns:ns3="7178be8b-d0ef-4995-97d9-396f4bad9a56" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="46a6dac1cb1c034944cf78d34111dc32" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -2213,33 +2239,33 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{704D0896-41A1-4D8E-B2B4-DAF4537F2CEF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="e7647ff1-e2f7-42a1-a68c-3c96587cf758"/>
+    <ds:schemaRef ds:uri="7178be8b-d0ef-4995-97d9-396f4bad9a56"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_Flow_SignoffStatus xmlns="e7647ff1-e2f7-42a1-a68c-3c96587cf758" xsi:nil="true"/>
-    <SharedWithUsers xmlns="7178be8b-d0ef-4995-97d9-396f4bad9a56">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{95702B07-5163-4733-93F0-15C1454EB37E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{169FD9BA-39C5-40E5-9D02-8D3DF9B0119E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2257,30 +2283,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{95702B07-5163-4733-93F0-15C1454EB37E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{704D0896-41A1-4D8E-B2B4-DAF4537F2CEF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="e7647ff1-e2f7-42a1-a68c-3c96587cf758"/>
-    <ds:schemaRef ds:uri="7178be8b-d0ef-4995-97d9-396f4bad9a56"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Implemented new house, has veranda. Additional textures have been applied
</commit_message>
<xml_diff>
--- a/CG_FinalAssignment_EvaluationForm_s1129160_LucasOuwens.xlsx
+++ b/CG_FinalAssignment_EvaluationForm_s1129160_LucasOuwens.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\School\CG_2021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBF4432A-DBF2-4FB7-AC5F-FF4BD06410C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C53D33C5-8DF7-484E-AAF2-3FA467E3C26E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Evaluation form" sheetId="1" r:id="rId1"/>
@@ -341,24 +341,12 @@
     <t>Only have a single mesh (but they fill the entire ground). It is also really easy to extend. (just create a new subclass &amp; add it)</t>
   </si>
   <si>
-    <t>floor grass texture, floor dirt texture, skybox texture, glass window texture, granite stone supports of fence texture, wooden fence texture, couch texture. Multiple textures are easily added by splitting a big model into smaller ones and applying a texture on them separately. Then we can easily group them together using a MeshGrouping</t>
-  </si>
-  <si>
     <t>Application of strategy pattern for movement controllers, code is documented. Modularity and code quality has been applied consistently.</t>
   </si>
   <si>
-    <t>Skybox, floor, two different trees, two different bushes, a house, a fence with a fence gate, a flower and a couch. I made all the models in the world by myself.</t>
-  </si>
-  <si>
     <t>Comments have been placed at their relevant locations, method and variable naming is clear. Note that methods are explained in the .h file &amp; not the .cpp file. This has been the most convenient way for me to add useful comments without adding duplicity.</t>
   </si>
   <si>
-    <t>Skybox, floor, two different trees, two different bushes, a house, a fence with a fence gate, a flower and a couch. You can easily expand the amount of models by writing some code in the geometrybuilder and environmentbuilder.</t>
-  </si>
-  <si>
-    <t>basic shading on the house, phong shading on the other objects. The further you are from (12, N, 32) the less shiny the floor is.</t>
-  </si>
-  <si>
     <t>Implemented drone mode, switching can be done by using 'v'. You will be transported upon applying it. You will get a nice overview of the scene, you can move around like a drone (camera moves towards where you are facing incl y-axis.) You can also use Q/E to move up and down if you prefer this.</t>
   </si>
   <si>
@@ -368,7 +356,19 @@
     <t>Easy to use animation system, just create a subclass, implement the execute method. Then, make a new object out of the animation and set the owner of the animation &amp; register it at the animation manager. Skybox rotates, flower moves up and back down whilst rotating on the y and x axis. Couches have wave animations for seats. Press 'g' to open/cose the gate of the fence, you can stop it from opening or closer further by prematurely pressing 'g' again. There are birds flying around, their wings flap and they move in a direction.</t>
   </si>
   <si>
-    <t>I believe I have made good looking objects. My scene is pretty creative, the birds flying, the shockwave couch, the openable fence gate, etc.</t>
+    <t>Skybox, floor, two different trees, two different bushes, a house, a veranda for that house, a fence with a fence gate, a flower and a couch. I made all the models in the world by myself.</t>
+  </si>
+  <si>
+    <t>Skybox, floor, two different trees, two different bushes, a house, a veranda for that house, a fence with a fence gate, a flower and a couch. You can easily expand the amount of models by writing some code in the geometrybuilder and environmentbuilder.</t>
+  </si>
+  <si>
+    <t>floor grass texture, floor dirt texture, floor road texture, skybox texture, glass window texture, granite stone supports of fence texture, wooden fence texture, couch texture, sunflower texture on flower, living tree leafs texture, house veranda floor texture, house veranda roof texture, and so on. Multiple textures are easily added by splitting a big model into smaller ones and applying a texture on them separately. Then we can easily group them together using a MeshGrouping.</t>
+  </si>
+  <si>
+    <t>basic shading on the house, lmabert shading on the stemmed bushes and phong shading on the other objects. The further you are from (12, N, 32) the less shiny the floor is.</t>
+  </si>
+  <si>
+    <t>I believe I have made good looking objects. My scene is pretty creative, the birds flying, the shockwave couch, the openable fence gate, the silly combination of textures, etc.</t>
   </si>
 </sst>
 </file>
@@ -1355,7 +1355,7 @@
   <dimension ref="B2:M36"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A29" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M36" sqref="M36"/>
+      <selection activeCell="J35" sqref="J35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1516,7 +1516,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="2:13" ht="105" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:13" ht="120" x14ac:dyDescent="0.25">
       <c r="C19" s="4" t="s">
         <v>84</v>
       </c>
@@ -1535,7 +1535,7 @@
         <v>64</v>
       </c>
       <c r="M19" s="31" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="20" spans="2:13" ht="60" x14ac:dyDescent="0.25">
@@ -1579,10 +1579,10 @@
         <v>49</v>
       </c>
       <c r="M21" s="32" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="22" spans="2:13" ht="150" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="22" spans="2:13" ht="210" x14ac:dyDescent="0.25">
       <c r="C22" s="4" t="s">
         <v>53</v>
       </c>
@@ -1601,7 +1601,7 @@
         <v>57</v>
       </c>
       <c r="M22" s="32" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
     </row>
     <row r="23" spans="2:13" ht="225" x14ac:dyDescent="0.25">
@@ -1623,10 +1623,10 @@
         <v>58</v>
       </c>
       <c r="M23" s="32" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="24" spans="2:13" ht="60" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="24" spans="2:13" ht="75" x14ac:dyDescent="0.25">
       <c r="C24" s="4" t="s">
         <v>82</v>
       </c>
@@ -1645,7 +1645,7 @@
         <v>81</v>
       </c>
       <c r="M24" s="32" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
     </row>
     <row r="25" spans="2:13" ht="60" x14ac:dyDescent="0.25">
@@ -1687,7 +1687,7 @@
       </c>
       <c r="K26" s="48"/>
       <c r="M26" s="33" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="28" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1736,7 +1736,7 @@
         <v>45</v>
       </c>
       <c r="M29" s="28" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="30" spans="2:13" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1758,7 +1758,7 @@
         <v>42</v>
       </c>
       <c r="M30" s="29" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="32" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1805,7 +1805,7 @@
       </c>
       <c r="K33" s="39"/>
       <c r="M33" s="28" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="34" spans="3:13" ht="30" x14ac:dyDescent="0.25">
@@ -1826,7 +1826,7 @@
       <c r="K34" s="39"/>
       <c r="M34" s="28"/>
     </row>
-    <row r="35" spans="3:13" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="3:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C35" s="4" t="s">
         <v>60</v>
       </c>

</xml_diff>

<commit_message>
Added primitive geometries & animated the spikes.
</commit_message>
<xml_diff>
--- a/CG_FinalAssignment_EvaluationForm_s1129160_LucasOuwens.xlsx
+++ b/CG_FinalAssignment_EvaluationForm_s1129160_LucasOuwens.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\School\CG_2021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6EFDC0F-ED48-4AF8-927A-A27344858DCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{955F2CDA-4175-4799-80D5-32A50055C5B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -350,9 +350,6 @@
     <t>My models look pretty decent, I believe.</t>
   </si>
   <si>
-    <t>Easy to use animation system, just create a subclass, implement the execute method. Then, make a new object out of the animation and set the owner of the animation &amp; register it at the animation manager. Skybox rotates, flower moves up and back down whilst rotating on the y and x axis. Couches have wave animations for seats. Press 'g' to open/cose the gate of the fence, you can stop it from opening or closer further by prematurely pressing 'g' again. There are birds flying around, their wings flap and they move in a direction.</t>
-  </si>
-  <si>
     <t>Skybox, floor, two different trees, two different bushes, a house, a veranda for that house, a fence with a fence gate, a flower and a couch. I made all the models in the world by myself.</t>
   </si>
   <si>
@@ -369,6 +366,9 @@
   </si>
   <si>
     <t>floor grass texture, floor dirt texture, floor road texture, skybox texture, glass window texture, granite stone supports of fence texture, wooden fence texture, couch texture, sunflower texture on flower, living tree leafs texture, house veranda floor texture, house veranda roof texture, and so on. There are many textures, not counting solid color textures. Multiple textures are easily added by splitting a big model into smaller ones and applying a texture on them separately. Then we can easily group them together using a MeshGrouping.</t>
+  </si>
+  <si>
+    <t>Easy to use animation system, just create a subclass, implement the execute method. Then, make a new object out of the animation and set the owner of the animation &amp; register it at the animation manager. Skybox rotates, flower moves up and back down whilst rotating on the y and x axis. Couches have wave animations for seats. Press 'g' to open/cose the gate of the fence, you can stop it from opening or closer further by prematurely pressing 'g' again. There are birds flying around, their wings flap and they move in a direction. The primitive spike trap's spikes also scale up/down.</t>
   </si>
 </sst>
 </file>
@@ -1355,7 +1355,7 @@
   <dimension ref="B2:M36"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A23" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+      <selection activeCell="M24" sqref="M24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1535,7 +1535,7 @@
         <v>64</v>
       </c>
       <c r="M19" s="31" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="20" spans="2:13" ht="135" x14ac:dyDescent="0.25">
@@ -1557,7 +1557,7 @@
         <v>87</v>
       </c>
       <c r="M20" s="32" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="21" spans="2:13" ht="75" x14ac:dyDescent="0.25">
@@ -1579,7 +1579,7 @@
         <v>49</v>
       </c>
       <c r="M21" s="32" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="22" spans="2:13" ht="240" x14ac:dyDescent="0.25">
@@ -1601,10 +1601,10 @@
         <v>57</v>
       </c>
       <c r="M22" s="32" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="23" spans="2:13" ht="225" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="23" spans="2:13" ht="255" x14ac:dyDescent="0.25">
       <c r="C23" s="4" t="s">
         <v>32</v>
       </c>
@@ -1623,7 +1623,7 @@
         <v>58</v>
       </c>
       <c r="M23" s="32" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
     </row>
     <row r="24" spans="2:13" ht="75" x14ac:dyDescent="0.25">
@@ -1645,7 +1645,7 @@
         <v>81</v>
       </c>
       <c r="M24" s="32" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="25" spans="2:13" ht="60" x14ac:dyDescent="0.25">
@@ -1845,7 +1845,7 @@
         <v>73</v>
       </c>
       <c r="M35" s="29" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="36" spans="3:13" x14ac:dyDescent="0.25">
@@ -1974,32 +1974,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_Flow_SignoffStatus xmlns="e7647ff1-e2f7-42a1-a68c-3c96587cf758" xsi:nil="true"/>
-    <SharedWithUsers xmlns="7178be8b-d0ef-4995-97d9-396f4bad9a56">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010031DCE2413392E94399C66D8B3C6C85EE" ma:contentTypeVersion="15" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="0c2036bf52fce6a572da55f07fac53b0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="e7647ff1-e2f7-42a1-a68c-3c96587cf758" xmlns:ns3="7178be8b-d0ef-4995-97d9-396f4bad9a56" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="46a6dac1cb1c034944cf78d34111dc32" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -2239,33 +2213,33 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{704D0896-41A1-4D8E-B2B4-DAF4537F2CEF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="e7647ff1-e2f7-42a1-a68c-3c96587cf758"/>
-    <ds:schemaRef ds:uri="7178be8b-d0ef-4995-97d9-396f4bad9a56"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{95702B07-5163-4733-93F0-15C1454EB37E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_Flow_SignoffStatus xmlns="e7647ff1-e2f7-42a1-a68c-3c96587cf758" xsi:nil="true"/>
+    <SharedWithUsers xmlns="7178be8b-d0ef-4995-97d9-396f4bad9a56">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{169FD9BA-39C5-40E5-9D02-8D3DF9B0119E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2283,4 +2257,30 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{95702B07-5163-4733-93F0-15C1454EB37E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{704D0896-41A1-4D8E-B2B4-DAF4537F2CEF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="e7647ff1-e2f7-42a1-a68c-3c96587cf758"/>
+    <ds:schemaRef ds:uri="7178be8b-d0ef-4995-97d9-396f4bad9a56"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>